<commit_message>
enhanced the last photo
</commit_message>
<xml_diff>
--- a/dataset/wider_face_style_train/retinaface_real_people.xlsx
+++ b/dataset/wider_face_style_train/retinaface_real_people.xlsx
@@ -438,19 +438,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>0.8758091609921949</v>
+        <v>0.8642207331115092</v>
       </c>
       <c r="B2">
-        <v>0.1456656715576808</v>
+        <v>0.1363113876655567</v>
       </c>
       <c r="C2">
-        <v>0.0303745236834077</v>
+        <v>0.04578119463364336</v>
       </c>
       <c r="D2">
-        <v>0.04972054423406965</v>
+        <v>0.05121405139420469</v>
       </c>
       <c r="E2">
-        <v>0.014182125375862</v>
+        <v>0.01281323918690157</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -458,19 +458,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>-0.7372671293692341</v>
+        <v>-0.7493438769507179</v>
       </c>
       <c r="B3">
-        <v>-0.1047591441959792</v>
+        <v>-0.1096752117862357</v>
       </c>
       <c r="C3">
-        <v>-0.1220359586953075</v>
+        <v>-0.1176799860765908</v>
       </c>
       <c r="D3">
-        <v>-0.05747342243201718</v>
+        <v>-0.06928264725392688</v>
       </c>
       <c r="E3">
-        <v>-0.06309294754189695</v>
+        <v>-0.03709190225500564</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -478,19 +478,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>0.8233883484984734</v>
+        <v>0.8079570140813407</v>
       </c>
       <c r="B4">
-        <v>-0.6702436551811957</v>
+        <v>-0.6854285361295791</v>
       </c>
       <c r="C4">
-        <v>-0.1907170890234385</v>
+        <v>-0.1563013979260822</v>
       </c>
       <c r="D4">
-        <v>-0.05462147583948596</v>
+        <v>-0.07103987200492272</v>
       </c>
       <c r="E4">
-        <v>0.4002078676408962</v>
+        <v>0.4063360846629895</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
@@ -498,19 +498,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>-1.165580149451538</v>
+        <v>-1.175609776417535</v>
       </c>
       <c r="B5">
-        <v>0.1555490989249321</v>
+        <v>0.1555520270486837</v>
       </c>
       <c r="C5">
-        <v>-0.05621166593046584</v>
+        <v>-0.0644464287667121</v>
       </c>
       <c r="D5">
-        <v>0.3544734625681717</v>
+        <v>0.3553363052157871</v>
       </c>
       <c r="E5">
-        <v>0.1210184007446644</v>
+        <v>0.1271337456501989</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -518,19 +518,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>0.0877798201780903</v>
+        <v>0.06495539128117102</v>
       </c>
       <c r="B6">
-        <v>0.06649421185651727</v>
+        <v>0.0789486889287169</v>
       </c>
       <c r="C6">
-        <v>1.008885445404731</v>
+        <v>1.018400170891542</v>
       </c>
       <c r="D6">
-        <v>-0.179416191020832</v>
+        <v>-0.1767022849442542</v>
       </c>
       <c r="E6">
-        <v>-0.1153018374881904</v>
+        <v>-0.1102773514992586</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -538,19 +538,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>0.7610674660724833</v>
+        <v>0.7522842474710878</v>
       </c>
       <c r="B7">
-        <v>0.520136978133844</v>
+        <v>0.507080248125388</v>
       </c>
       <c r="C7">
-        <v>-0.1204839248497289</v>
+        <v>-0.1112064084468449</v>
       </c>
       <c r="D7">
-        <v>-0.1841686725234966</v>
+        <v>-0.1840062700387655</v>
       </c>
       <c r="E7">
-        <v>-0.02616786726344315</v>
+        <v>-0.03259610385937829</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -558,19 +558,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>-1.368391369256041</v>
+        <v>-1.384045075172148</v>
       </c>
       <c r="B8">
-        <v>0.4939945435565279</v>
+        <v>0.5051798620542988</v>
       </c>
       <c r="C8">
-        <v>0.5580234993769727</v>
+        <v>0.5434878960052636</v>
       </c>
       <c r="D8">
-        <v>0.1399835491499147</v>
+        <v>0.139412633571673</v>
       </c>
       <c r="E8">
-        <v>0.1491676919940072</v>
+        <v>0.1543618289537597</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
@@ -578,19 +578,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>1.408032940467841</v>
+        <v>1.395546064300245</v>
       </c>
       <c r="B9">
-        <v>0.2493024717873551</v>
+        <v>0.2426975624373594</v>
       </c>
       <c r="C9">
-        <v>0.2531173200915994</v>
+        <v>0.2700753963239798</v>
       </c>
       <c r="D9">
-        <v>0.1462378969829151</v>
+        <v>0.1565944220195196</v>
       </c>
       <c r="E9">
-        <v>-0.1161123772501232</v>
+        <v>-0.1222780515201706</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
@@ -598,19 +598,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>1.096119895439053</v>
+        <v>1.083194354871956</v>
       </c>
       <c r="B10">
-        <v>0.36826299099001</v>
+        <v>0.3609484615105997</v>
       </c>
       <c r="C10">
-        <v>0.2244615154982648</v>
+        <v>0.2389046647733641</v>
       </c>
       <c r="D10">
-        <v>0.04292530331140672</v>
+        <v>0.0438269765960545</v>
       </c>
       <c r="E10">
-        <v>0.1010948182492413</v>
+        <v>0.09610876909250834</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -618,19 +618,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>-0.1067357895442648</v>
+        <v>-0.1181627099546504</v>
       </c>
       <c r="B11">
-        <v>-0.8420521371543028</v>
+        <v>-0.8565148948013409</v>
       </c>
       <c r="C11">
-        <v>-0.4719556162808553</v>
+        <v>-0.4473494836059416</v>
       </c>
       <c r="D11">
-        <v>-0.1020605679245228</v>
+        <v>-0.09655150832614325</v>
       </c>
       <c r="E11">
-        <v>-0.0798600964354471</v>
+        <v>-0.0848394904264534</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -638,19 +638,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>-0.2217306744017034</v>
+        <v>-0.229075450112245</v>
       </c>
       <c r="B12">
-        <v>-0.2200294021399054</v>
+        <v>-0.2348543394962437</v>
       </c>
       <c r="C12">
-        <v>-0.5423054772369749</v>
+        <v>-0.5315286909402757</v>
       </c>
       <c r="D12">
-        <v>0.008169153519337729</v>
+        <v>0.007715732159584824</v>
       </c>
       <c r="E12">
-        <v>-0.06628549662835299</v>
+        <v>-0.06202599751200395</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -658,19 +658,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>0.3343190540355936</v>
+        <v>0.5543787745226978</v>
       </c>
       <c r="B13">
-        <v>-0.1115530872198304</v>
+        <v>-0.003181651446204666</v>
       </c>
       <c r="C13">
-        <v>0.05343509026076672</v>
+        <v>-0.1137064838100931</v>
       </c>
       <c r="D13">
-        <v>0.2030678045248385</v>
+        <v>0.1960103572456168</v>
       </c>
       <c r="E13">
-        <v>-0.1514931907215794</v>
+        <v>-0.1664810034022458</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -678,19 +678,19 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>-0.8988670880536664</v>
+        <v>-0.8978468511190866</v>
       </c>
       <c r="B14">
-        <v>1.143145742661293</v>
+        <v>1.124684196671407</v>
       </c>
       <c r="C14">
-        <v>-0.7944206798352704</v>
+        <v>-0.8134283426685033</v>
       </c>
       <c r="D14">
-        <v>-0.2208169693103831</v>
+        <v>-0.2248840478160939</v>
       </c>
       <c r="E14">
-        <v>0.05659203663766033</v>
+        <v>0.04070928574358189</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -698,19 +698,19 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>-1.190326877979055</v>
+        <v>-1.214267130075492</v>
       </c>
       <c r="B15">
-        <v>-0.6394644963598778</v>
+        <v>-0.6254253284497149</v>
       </c>
       <c r="C15">
-        <v>0.8361680282062736</v>
+        <v>0.8469811931058914</v>
       </c>
       <c r="D15">
-        <v>-0.2263763628029714</v>
+        <v>-0.1875940324736835</v>
       </c>
       <c r="E15">
-        <v>0.01429300223526748</v>
+        <v>-0.04128058367036361</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -718,19 +718,19 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>-0.07525117093650839</v>
+        <v>-0.08946275117270334</v>
       </c>
       <c r="B16">
-        <v>0.03377413674262371</v>
+        <v>0.03441640488013157</v>
       </c>
       <c r="C16">
-        <v>0.263540026631381</v>
+        <v>0.2694810031973771</v>
       </c>
       <c r="D16">
-        <v>0.1131841965203469</v>
+        <v>0.1116597438947088</v>
       </c>
       <c r="E16">
-        <v>-0.07954422218232801</v>
+        <v>-0.06546902300932564</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -738,19 +738,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>-0.2051745023951163</v>
+        <v>-0.2147352042717159</v>
       </c>
       <c r="B17">
-        <v>-0.6746121598014183</v>
+        <v>-0.6875542951599238</v>
       </c>
       <c r="C17">
-        <v>-0.4784486507106828</v>
+        <v>-0.4602597451216613</v>
       </c>
       <c r="D17">
-        <v>0.1275212015294543</v>
+        <v>0.1389837810984315</v>
       </c>
       <c r="E17">
-        <v>-0.05081056579688434</v>
+        <v>-0.06124221788119844</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
@@ -758,19 +758,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>0.2336893977173727</v>
+        <v>0.2231560037435797</v>
       </c>
       <c r="B18">
-        <v>0.2068665248022683</v>
+        <v>0.199329442381917</v>
       </c>
       <c r="C18">
-        <v>-0.04895075550851506</v>
+        <v>-0.04170985658668373</v>
       </c>
       <c r="D18">
-        <v>0.006164091190530642</v>
+        <v>0.0006629232391801249</v>
       </c>
       <c r="E18">
-        <v>-0.1011361581829439</v>
+        <v>-0.08558345381585487</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
@@ -778,19 +778,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>-0.3179499567722147</v>
+        <v>-0.3261270174712719</v>
       </c>
       <c r="B19">
-        <v>-0.1107669705322763</v>
+        <v>-0.1233073540643913</v>
       </c>
       <c r="C19">
-        <v>-0.4401651963521437</v>
+        <v>-0.432155590577181</v>
       </c>
       <c r="D19">
-        <v>-0.06713408390387306</v>
+        <v>-0.07398362606105821</v>
       </c>
       <c r="E19">
-        <v>-0.1486898106091275</v>
+        <v>-0.1307643344056267</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -798,19 +798,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>0.66706862475824</v>
+        <v>0.6529832593339772</v>
       </c>
       <c r="B20">
-        <v>-0.009711318428266447</v>
+        <v>-0.01920667037042418</v>
       </c>
       <c r="C20">
-        <v>0.03768956526998524</v>
+        <v>0.0566608955955071</v>
       </c>
       <c r="D20">
-        <v>-0.09937945777340564</v>
+        <v>-0.1173726375159124</v>
       </c>
       <c r="E20">
-        <v>0.1419386272227186</v>
+        <v>0.1624665599669474</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>

</xml_diff>